<commit_message>
Correct Tests. Fix Camera Roll error when no photos. Point work.
</commit_message>
<xml_diff>
--- a/PointlessWaymarksTests/IronwoodTestContent/GrandCanyonPointsImport.xlsx
+++ b/PointlessWaymarksTests/IronwoodTestContent/GrandCanyonPointsImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PointlessWaymarksCms05\PointlessWaymarksTests\IronwoodTestContent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE64FF4-EB0C-43DD-9949-08ECEFA5A754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B81FD2-E5B3-415A-9570-B12E13A8FDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="25600" windowHeight="13760" xr2:uid="{A502E4A2-19B3-43B1-97B2-6120C4E9A4F5}"/>
   </bookViews>
@@ -1219,6 +1219,14 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1259,13 +1267,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1647,24 +1648,24 @@
     <tableColumn id="27" xr3:uid="{E609B391-60DB-4FD0-BA56-92ECCFD26CDC}" name="Latitude" dataDxfId="10">
       <calculatedColumnFormula>J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{3EB02439-D402-4820-A58D-32055C4FB187}" name="Longitude" dataDxfId="9">
-      <calculatedColumnFormula>J2</calculatedColumnFormula>
+    <tableColumn id="28" xr3:uid="{3EB02439-D402-4820-A58D-32055C4FB187}" name="Longitude" dataDxfId="0">
+      <calculatedColumnFormula>K2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{57726F3C-3D0A-4F88-8A54-44F1D05E6C01}" name="Elevation" dataDxfId="8">
+    <tableColumn id="29" xr3:uid="{57726F3C-3D0A-4F88-8A54-44F1D05E6C01}" name="Elevation" dataDxfId="9">
       <calculatedColumnFormula>Q2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{8F20A88D-6858-45A4-8E38-F19B00355AE2}" name="Folder" dataDxfId="7"/>
-    <tableColumn id="31" xr3:uid="{3EC3ADE0-E440-4A7E-A232-87920FE0EF97}" name="ShowInMainSiteFeed" dataDxfId="6"/>
-    <tableColumn id="32" xr3:uid="{ED042FF5-C765-41B2-A54A-1095F3ED4444}" name="Summary" dataDxfId="5">
+    <tableColumn id="30" xr3:uid="{8F20A88D-6858-45A4-8E38-F19B00355AE2}" name="Folder" dataDxfId="8"/>
+    <tableColumn id="31" xr3:uid="{3EC3ADE0-E440-4A7E-A232-87920FE0EF97}" name="ShowInMainSiteFeed" dataDxfId="7"/>
+    <tableColumn id="32" xr3:uid="{ED042FF5-C765-41B2-A54A-1095F3ED4444}" name="Summary" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(B2,", ",F2," County, ",D2,"."," USGS 7.5' Map: ", R2,".")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{83B88F62-B46F-4CED-A530-3B101E8CBBFA}" name="Tags" dataDxfId="4">
+    <tableColumn id="33" xr3:uid="{83B88F62-B46F-4CED-A530-3B101E8CBBFA}" name="Tags" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.CONCAT("grand canyon, ", B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{6B0E8F35-25DB-4BD6-93F3-2E2E8DBACA78}" name="CreatedBy" dataDxfId="3"/>
-    <tableColumn id="35" xr3:uid="{2CCAFA83-E69E-4E91-92D8-DF4C6DC8F9FC}" name="CreatedOn" dataDxfId="2"/>
-    <tableColumn id="36" xr3:uid="{DEE1C7CE-9A12-46E0-B3F8-8B00D65FFA10}" name="UpdateContentFormat" dataDxfId="1"/>
-    <tableColumn id="37" xr3:uid="{83A7D6D9-9F51-4C21-A2CB-179160B8B0D4}" name="PointDetail 1" dataDxfId="0">
+    <tableColumn id="34" xr3:uid="{6B0E8F35-25DB-4BD6-93F3-2E2E8DBACA78}" name="CreatedBy" dataDxfId="4"/>
+    <tableColumn id="35" xr3:uid="{2CCAFA83-E69E-4E91-92D8-DF4C6DC8F9FC}" name="CreatedOn" dataDxfId="3"/>
+    <tableColumn id="36" xr3:uid="{DEE1C7CE-9A12-46E0-B3F8-8B00D65FFA10}" name="UpdateContentFormat" dataDxfId="2"/>
+    <tableColumn id="37" xr3:uid="{83A7D6D9-9F51-4C21-A2CB-179160B8B0D4}" name="PointDetail 1" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("ContentId:||Type:Feature||Data:{""DataTypeIdentifier"":""Feature"",""Type"":""",C2,""",""Notes"":""GNIS Feature ID:",A2,", ", F2," County, ",D2,". USGS 7.5' Quad: ",R2,". GNIS Elevation: ", Q2,"'. GNIS Entry Created: ", TEXT(S2,"M/D/YYYY"),IF(ISBLANK(T2),".",_xlfn.CONCAT(", Updated: ", TEXT(T2,"M/D/YYYY"),". ")),"""}")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1971,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5FEDEF-5A8E-421A-8857-D6C400357593}">
   <dimension ref="A1:AK99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2203,8 +2204,8 @@
         <v>36.094258000000004</v>
       </c>
       <c r="AB2" s="2">
-        <f t="shared" ref="AB2:AB33" si="3">J2</f>
-        <v>36.094258000000004</v>
+        <f t="shared" ref="AB2:AB33" si="3">K2</f>
+        <v>-112.37395840000001</v>
       </c>
       <c r="AC2" s="2">
         <f t="shared" ref="AC2:AC33" si="4">Q2</f>
@@ -2321,7 +2322,7 @@
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="3"/>
-        <v>36.115259600000002</v>
+        <v>-112.230728</v>
       </c>
       <c r="AC3" s="2">
         <f t="shared" si="4"/>
@@ -2432,7 +2433,7 @@
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="3"/>
-        <v>36.1163417</v>
+        <v>-112.2299957</v>
       </c>
       <c r="AC4" s="2">
         <f t="shared" si="4"/>
@@ -2541,7 +2542,7 @@
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="3"/>
-        <v>36.080260199999998</v>
+        <v>-112.2026714</v>
       </c>
       <c r="AC5" s="2">
         <f t="shared" si="4"/>
@@ -2652,7 +2653,7 @@
       </c>
       <c r="AB6" s="2">
         <f t="shared" si="3"/>
-        <v>36.069149500000002</v>
+        <v>-112.1329471</v>
       </c>
       <c r="AC6" s="2">
         <f t="shared" si="4"/>
@@ -2769,7 +2770,7 @@
       </c>
       <c r="AB7" s="2">
         <f t="shared" si="3"/>
-        <v>36.003594300000003</v>
+        <v>-112.2112822</v>
       </c>
       <c r="AC7" s="2">
         <f t="shared" si="4"/>
@@ -2880,7 +2881,7 @@
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="3"/>
-        <v>36.009662499999997</v>
+        <v>-112.2425102</v>
       </c>
       <c r="AC8" s="2">
         <f t="shared" si="4"/>
@@ -2989,7 +2990,7 @@
       </c>
       <c r="AB9" s="2">
         <f t="shared" si="3"/>
-        <v>36.081371300000001</v>
+        <v>-112.19878249999999</v>
       </c>
       <c r="AC9" s="2">
         <f t="shared" si="4"/>
@@ -3100,7 +3101,7 @@
       </c>
       <c r="AB10" s="2">
         <f t="shared" si="3"/>
-        <v>36.088920999999999</v>
+        <v>-112.178173</v>
       </c>
       <c r="AC10" s="2">
         <f t="shared" si="4"/>
@@ -3209,7 +3210,7 @@
       </c>
       <c r="AB11" s="2">
         <f t="shared" si="3"/>
-        <v>36.088037700000001</v>
+        <v>-112.2460061</v>
       </c>
       <c r="AC11" s="2">
         <f t="shared" si="4"/>
@@ -3318,7 +3319,7 @@
       </c>
       <c r="AB12" s="2">
         <f t="shared" si="3"/>
-        <v>36.083037900000001</v>
+        <v>-112.2198942</v>
       </c>
       <c r="AC12" s="2">
         <f t="shared" si="4"/>
@@ -3429,7 +3430,7 @@
       </c>
       <c r="AB13" s="2">
         <f t="shared" si="3"/>
-        <v>36.087649900000002</v>
+        <v>-112.1973931</v>
       </c>
       <c r="AC13" s="2">
         <f t="shared" si="4"/>
@@ -3540,7 +3541,7 @@
       </c>
       <c r="AB14" s="2">
         <f t="shared" si="3"/>
-        <v>36.091582799999998</v>
+        <v>-112.15024339999999</v>
       </c>
       <c r="AC14" s="2">
         <f t="shared" si="4"/>
@@ -3651,7 +3652,7 @@
       </c>
       <c r="AB15" s="2">
         <f t="shared" si="3"/>
-        <v>36.1118071</v>
+        <v>-112.270048</v>
       </c>
       <c r="AC15" s="2">
         <f t="shared" si="4"/>
@@ -3762,7 +3763,7 @@
       </c>
       <c r="AB16" s="2">
         <f t="shared" si="3"/>
-        <v>36.062370799999997</v>
+        <v>-112.2422765</v>
       </c>
       <c r="AC16" s="2">
         <f t="shared" si="4"/>
@@ -3871,7 +3872,7 @@
       </c>
       <c r="AB17" s="2">
         <f t="shared" si="3"/>
-        <v>36.060260300000003</v>
+        <v>-112.2404501</v>
       </c>
       <c r="AC17" s="2">
         <f t="shared" si="4"/>
@@ -3982,7 +3983,7 @@
       </c>
       <c r="AB18" s="2">
         <f t="shared" si="3"/>
-        <v>36.076015200000001</v>
+        <v>-112.2314057</v>
       </c>
       <c r="AC18" s="2">
         <f t="shared" si="4"/>
@@ -4093,7 +4094,7 @@
       </c>
       <c r="AB19" s="2">
         <f t="shared" si="3"/>
-        <v>36.071687599999997</v>
+        <v>-112.2542091</v>
       </c>
       <c r="AC19" s="2">
         <f t="shared" si="4"/>
@@ -4202,7 +4203,7 @@
       </c>
       <c r="AB20" s="2">
         <f t="shared" si="3"/>
-        <v>36.0738713</v>
+        <v>-112.2101715</v>
       </c>
       <c r="AC20" s="2">
         <f t="shared" si="4"/>
@@ -4313,7 +4314,7 @@
       </c>
       <c r="AB21" s="2">
         <f t="shared" si="3"/>
-        <v>36.0544273</v>
+        <v>-112.139336</v>
       </c>
       <c r="AC21" s="2">
         <f t="shared" si="4"/>
@@ -4424,7 +4425,7 @@
       </c>
       <c r="AB22" s="2">
         <f t="shared" si="3"/>
-        <v>36.098559000000002</v>
+        <v>-112.18359649999999</v>
       </c>
       <c r="AC22" s="2">
         <f t="shared" si="4"/>
@@ -4533,7 +4534,7 @@
       </c>
       <c r="AB23" s="2">
         <f t="shared" si="3"/>
-        <v>36.063038300000002</v>
+        <v>-112.1698926</v>
       </c>
       <c r="AC23" s="2">
         <f t="shared" si="4"/>
@@ -4650,7 +4651,7 @@
       </c>
       <c r="AB24" s="2">
         <f t="shared" si="3"/>
-        <v>36.099148900000003</v>
+        <v>-112.2096162</v>
       </c>
       <c r="AC24" s="2">
         <f t="shared" si="4"/>
@@ -4761,7 +4762,7 @@
       </c>
       <c r="AB25" s="2">
         <f t="shared" si="3"/>
-        <v>36.100281099999997</v>
+        <v>-112.2103865</v>
       </c>
       <c r="AC25" s="2">
         <f t="shared" si="4"/>
@@ -4870,7 +4871,7 @@
       </c>
       <c r="AB26" s="2">
         <f t="shared" si="3"/>
-        <v>36.068038100000003</v>
+        <v>-112.2137828</v>
       </c>
       <c r="AC26" s="2">
         <f t="shared" si="4"/>
@@ -4979,7 +4980,7 @@
       </c>
       <c r="AB27" s="2">
         <f t="shared" si="3"/>
-        <v>36.061926999999997</v>
+        <v>-112.21100490000001</v>
       </c>
       <c r="AC27" s="2">
         <f t="shared" si="4"/>
@@ -5090,7 +5091,7 @@
       </c>
       <c r="AB28" s="2">
         <f t="shared" si="3"/>
-        <v>36.071514200000003</v>
+        <v>-112.34033100000001</v>
       </c>
       <c r="AC28" s="2">
         <f t="shared" si="4"/>
@@ -5199,7 +5200,7 @@
       </c>
       <c r="AB29" s="2">
         <f t="shared" si="3"/>
-        <v>36.076093800000002</v>
+        <v>-112.15461449999999</v>
       </c>
       <c r="AC29" s="2">
         <f t="shared" si="4"/>
@@ -5310,7 +5311,7 @@
       </c>
       <c r="AB30" s="2">
         <f t="shared" si="3"/>
-        <v>36.069704899999998</v>
+        <v>-112.161559</v>
       </c>
       <c r="AC30" s="2">
         <f t="shared" si="4"/>
@@ -5427,7 +5428,7 @@
       </c>
       <c r="AB31" s="2">
         <f t="shared" si="3"/>
-        <v>36.098871500000001</v>
+        <v>-112.13489199999999</v>
       </c>
       <c r="AC31" s="2">
         <f t="shared" si="4"/>
@@ -5538,7 +5539,7 @@
       </c>
       <c r="AB32" s="2">
         <f t="shared" si="3"/>
-        <v>36.099516700000002</v>
+        <v>-112.1347811</v>
       </c>
       <c r="AC32" s="2">
         <f t="shared" si="4"/>
@@ -5649,7 +5650,7 @@
       </c>
       <c r="AB33" s="2">
         <f t="shared" si="3"/>
-        <v>36.039820300000002</v>
+        <v>-112.22014799999999</v>
       </c>
       <c r="AC33" s="2">
         <f t="shared" si="4"/>
@@ -5759,8 +5760,8 @@
         <v>36.013239800000001</v>
       </c>
       <c r="AB34" s="2">
-        <f t="shared" ref="AB34:AB65" si="11">J34</f>
-        <v>36.013239800000001</v>
+        <f t="shared" ref="AB34:AB65" si="11">K34</f>
+        <v>-112.2771415</v>
       </c>
       <c r="AC34" s="2">
         <f t="shared" ref="AC34:AC65" si="12">Q34</f>
@@ -5869,7 +5870,7 @@
       </c>
       <c r="AB35" s="2">
         <f t="shared" si="11"/>
-        <v>36.107759799999997</v>
+        <v>-112.31239739999999</v>
       </c>
       <c r="AC35" s="2">
         <f t="shared" si="12"/>
@@ -5980,7 +5981,7 @@
       </c>
       <c r="AB36" s="2">
         <f t="shared" si="11"/>
-        <v>36.0128384</v>
+        <v>-112.29757960000001</v>
       </c>
       <c r="AC36" s="2">
         <f t="shared" si="12"/>
@@ -6089,7 +6090,7 @@
       </c>
       <c r="AB37" s="2">
         <f t="shared" si="11"/>
-        <v>36.074982400000003</v>
+        <v>-112.2123939</v>
       </c>
       <c r="AC37" s="2">
         <f t="shared" si="12"/>
@@ -6198,7 +6199,7 @@
       </c>
       <c r="AB38" s="2">
         <f t="shared" si="11"/>
-        <v>36.069982799999998</v>
+        <v>-112.14628089999999</v>
       </c>
       <c r="AC38" s="2">
         <f t="shared" si="12"/>
@@ -6309,7 +6310,7 @@
       </c>
       <c r="AB39" s="2">
         <f t="shared" si="11"/>
-        <v>36.120731200000002</v>
+        <v>-112.24514019999999</v>
       </c>
       <c r="AC39" s="2">
         <f t="shared" si="12"/>
@@ -6418,7 +6419,7 @@
       </c>
       <c r="AB40" s="2">
         <f t="shared" si="11"/>
-        <v>36.1010931</v>
+        <v>-112.2893409</v>
       </c>
       <c r="AC40" s="2">
         <f t="shared" si="12"/>
@@ -6529,7 +6530,7 @@
       </c>
       <c r="AB41" s="2">
         <f t="shared" si="11"/>
-        <v>36.052044500000001</v>
+        <v>-112.3474171</v>
       </c>
       <c r="AC41" s="2">
         <f t="shared" si="12"/>
@@ -6640,7 +6641,7 @@
       </c>
       <c r="AB42" s="2">
         <f t="shared" si="11"/>
-        <v>36.062161000000003</v>
+        <v>-112.34783609999999</v>
       </c>
       <c r="AC42" s="2">
         <f t="shared" si="12"/>
@@ -6749,7 +6750,7 @@
       </c>
       <c r="AB43" s="2">
         <f t="shared" si="11"/>
-        <v>36.086371100000001</v>
+        <v>-112.2796183</v>
       </c>
       <c r="AC43" s="2">
         <f t="shared" si="12"/>
@@ -6858,7 +6859,7 @@
       </c>
       <c r="AB44" s="2">
         <f t="shared" si="11"/>
-        <v>36.072204900000003</v>
+        <v>-112.1660037</v>
       </c>
       <c r="AC44" s="2">
         <f t="shared" si="12"/>
@@ -6975,7 +6976,7 @@
       </c>
       <c r="AB45" s="2">
         <f t="shared" si="11"/>
-        <v>36.097760100000002</v>
+        <v>-112.18294880000001</v>
       </c>
       <c r="AC45" s="2">
         <f t="shared" si="12"/>
@@ -7086,7 +7087,7 @@
       </c>
       <c r="AB46" s="2">
         <f t="shared" si="11"/>
-        <v>36.0421768</v>
+        <v>-112.36173460000001</v>
       </c>
       <c r="AC46" s="2">
         <f t="shared" si="12"/>
@@ -7203,7 +7204,7 @@
       </c>
       <c r="AB47" s="2">
         <f t="shared" si="11"/>
-        <v>36.097204400000003</v>
+        <v>-112.1987826</v>
       </c>
       <c r="AC47" s="2">
         <f t="shared" si="12"/>
@@ -7320,7 +7321,7 @@
       </c>
       <c r="AB48" s="2">
         <f t="shared" si="11"/>
-        <v>36.1063714</v>
+        <v>-112.14711459999999</v>
       </c>
       <c r="AC48" s="2">
         <f t="shared" si="12"/>
@@ -7430,7 +7431,7 @@
       </c>
       <c r="AB49" s="2">
         <f t="shared" si="11"/>
-        <v>36.005865999999997</v>
+        <v>-112.24558620000001</v>
       </c>
       <c r="AC49" s="2">
         <f t="shared" si="12"/>
@@ -7541,7 +7542,7 @@
       </c>
       <c r="AB50" s="2">
         <f t="shared" si="11"/>
-        <v>36.071926900000001</v>
+        <v>-112.2001712</v>
       </c>
       <c r="AC50" s="2">
         <f t="shared" si="12"/>
@@ -7650,7 +7651,7 @@
       </c>
       <c r="AB51" s="2">
         <f t="shared" si="11"/>
-        <v>36.117759700000001</v>
+        <v>-112.32573120000001</v>
       </c>
       <c r="AC51" s="2">
         <f t="shared" si="12"/>
@@ -7761,7 +7762,7 @@
       </c>
       <c r="AB52" s="2">
         <f t="shared" si="11"/>
-        <v>36.120635900000003</v>
+        <v>-112.30257779999999</v>
       </c>
       <c r="AC52" s="2">
         <f t="shared" si="12"/>
@@ -7870,7 +7871,7 @@
       </c>
       <c r="AB53" s="2">
         <f t="shared" si="11"/>
-        <v>36.0747049</v>
+        <v>-112.1521144</v>
       </c>
       <c r="AC53" s="2">
         <f t="shared" si="12"/>
@@ -7981,7 +7982,7 @@
       </c>
       <c r="AB54" s="2">
         <f t="shared" si="11"/>
-        <v>36.034427299999997</v>
+        <v>-112.18044810000001</v>
       </c>
       <c r="AC54" s="2">
         <f t="shared" si="12"/>
@@ -8098,7 +8099,7 @@
       </c>
       <c r="AB55" s="2">
         <f t="shared" si="11"/>
-        <v>36.0985935</v>
+        <v>-112.1696151</v>
       </c>
       <c r="AC55" s="2">
         <f t="shared" si="12"/>
@@ -8209,7 +8210,7 @@
       </c>
       <c r="AB56" s="2">
         <f t="shared" si="11"/>
-        <v>36.099610499999997</v>
+        <v>-112.1704216</v>
       </c>
       <c r="AC56" s="2">
         <f t="shared" si="12"/>
@@ -8320,7 +8321,7 @@
       </c>
       <c r="AB57" s="2">
         <f t="shared" si="11"/>
-        <v>36.037934700000001</v>
+        <v>-112.298069</v>
       </c>
       <c r="AC57" s="2">
         <f t="shared" si="12"/>
@@ -8431,7 +8432,7 @@
       </c>
       <c r="AB58" s="2">
         <f t="shared" si="11"/>
-        <v>36.060098099999998</v>
+        <v>-112.2216801</v>
       </c>
       <c r="AC58" s="2">
         <f t="shared" si="12"/>
@@ -8542,7 +8543,7 @@
       </c>
       <c r="AB59" s="2">
         <f t="shared" si="11"/>
-        <v>36.104914000000001</v>
+        <v>-112.3563655</v>
       </c>
       <c r="AC59" s="2">
         <f t="shared" si="12"/>
@@ -8653,7 +8654,7 @@
       </c>
       <c r="AB60" s="2">
         <f t="shared" si="11"/>
-        <v>36.059297700000002</v>
+        <v>-112.3210589</v>
       </c>
       <c r="AC60" s="2">
         <f t="shared" si="12"/>
@@ -8762,7 +8763,7 @@
       </c>
       <c r="AB61" s="2">
         <f t="shared" si="11"/>
-        <v>36.078593699999999</v>
+        <v>-112.16933710000001</v>
       </c>
       <c r="AC61" s="2">
         <f t="shared" si="12"/>
@@ -8873,7 +8874,7 @@
       </c>
       <c r="AB62" s="2">
         <f t="shared" si="11"/>
-        <v>36.075827799999999</v>
+        <v>-112.1384702</v>
       </c>
       <c r="AC62" s="2">
         <f t="shared" si="12"/>
@@ -8984,7 +8985,7 @@
       </c>
       <c r="AB63" s="2">
         <f t="shared" si="11"/>
-        <v>36.077204799999997</v>
+        <v>-112.1621147</v>
       </c>
       <c r="AC63" s="2">
         <f t="shared" si="12"/>
@@ -9095,7 +9096,7 @@
       </c>
       <c r="AB64" s="2">
         <f t="shared" si="11"/>
-        <v>36.049502400000002</v>
+        <v>-112.3734821</v>
       </c>
       <c r="AC64" s="2">
         <f t="shared" si="12"/>
@@ -9214,7 +9215,7 @@
       </c>
       <c r="AB65" s="2">
         <f t="shared" si="11"/>
-        <v>36.110504499999998</v>
+        <v>-112.2407559</v>
       </c>
       <c r="AC65" s="2">
         <f t="shared" si="12"/>
@@ -9324,8 +9325,8 @@
         <v>36.121130600000001</v>
       </c>
       <c r="AB66" s="2">
-        <f t="shared" ref="AB66:AB99" si="18">J66</f>
-        <v>36.121130600000001</v>
+        <f t="shared" ref="AB66:AB99" si="18">K66</f>
+        <v>-112.1780426</v>
       </c>
       <c r="AC66" s="2">
         <f t="shared" ref="AC66:AC99" si="19">Q66</f>
@@ -9444,7 +9445,7 @@
       </c>
       <c r="AB67" s="2">
         <f t="shared" si="18"/>
-        <v>36.102882999999999</v>
+        <v>-112.2189362</v>
       </c>
       <c r="AC67" s="2">
         <f t="shared" si="19"/>
@@ -9561,7 +9562,7 @@
       </c>
       <c r="AB68" s="2">
         <f t="shared" si="18"/>
-        <v>36.1060935</v>
+        <v>-112.1532258</v>
       </c>
       <c r="AC68" s="2">
         <f t="shared" si="19"/>
@@ -9672,7 +9673,7 @@
       </c>
       <c r="AB69" s="2">
         <f t="shared" si="18"/>
-        <v>36.093509599999997</v>
+        <v>-112.2689987</v>
       </c>
       <c r="AC69" s="2">
         <f t="shared" si="19"/>
@@ -9783,7 +9784,7 @@
       </c>
       <c r="AB70" s="2">
         <f t="shared" si="18"/>
-        <v>36.097598300000001</v>
+        <v>-112.23120659999999</v>
       </c>
       <c r="AC70" s="2">
         <f t="shared" si="19"/>
@@ -9892,7 +9893,7 @@
       </c>
       <c r="AB71" s="2">
         <f t="shared" si="18"/>
-        <v>36.002761</v>
+        <v>-112.1957261</v>
       </c>
       <c r="AC71" s="2">
         <f t="shared" si="19"/>
@@ -10003,7 +10004,7 @@
       </c>
       <c r="AB72" s="2">
         <f t="shared" si="18"/>
-        <v>36.052439700000001</v>
+        <v>-112.1382175</v>
       </c>
       <c r="AC72" s="2">
         <f t="shared" si="19"/>
@@ -10114,7 +10115,7 @@
       </c>
       <c r="AB73" s="2">
         <f t="shared" si="18"/>
-        <v>36.0523284</v>
+        <v>-112.13865300000001</v>
       </c>
       <c r="AC73" s="2">
         <f t="shared" si="19"/>
@@ -10225,7 +10226,7 @@
       </c>
       <c r="AB74" s="2">
         <f t="shared" si="18"/>
-        <v>36.047859199999998</v>
+        <v>-112.1287932</v>
       </c>
       <c r="AC74" s="2">
         <f t="shared" si="19"/>
@@ -10336,7 +10337,7 @@
       </c>
       <c r="AB75" s="2">
         <f t="shared" si="18"/>
-        <v>36.056939999999997</v>
+        <v>-112.13667</v>
       </c>
       <c r="AC75" s="2">
         <f t="shared" si="19"/>
@@ -10445,7 +10446,7 @@
       </c>
       <c r="AB76" s="2">
         <f t="shared" si="18"/>
-        <v>36.050538199999998</v>
+        <v>-112.2198939</v>
       </c>
       <c r="AC76" s="2">
         <f t="shared" si="19"/>
@@ -10554,7 +10555,7 @@
       </c>
       <c r="AB77" s="2">
         <f t="shared" si="18"/>
-        <v>36.049705199999998</v>
+        <v>-112.13294689999999</v>
       </c>
       <c r="AC77" s="2">
         <f t="shared" si="19"/>
@@ -10665,7 +10666,7 @@
       </c>
       <c r="AB78" s="2">
         <f t="shared" si="18"/>
-        <v>36.0078198</v>
+        <v>-112.2061508</v>
       </c>
       <c r="AC78" s="2">
         <f t="shared" si="19"/>
@@ -10774,7 +10775,7 @@
       </c>
       <c r="AB79" s="2">
         <f t="shared" si="18"/>
-        <v>36.031371900000003</v>
+        <v>-112.174059</v>
       </c>
       <c r="AC79" s="2">
         <f t="shared" si="19"/>
@@ -10883,7 +10884,7 @@
       </c>
       <c r="AB80" s="2">
         <f t="shared" si="18"/>
-        <v>36.033871900000001</v>
+        <v>-112.1790592</v>
       </c>
       <c r="AC80" s="2">
         <f t="shared" si="19"/>
@@ -10994,7 +10995,7 @@
       </c>
       <c r="AB81" s="2">
         <f t="shared" si="18"/>
-        <v>36.0194106</v>
+        <v>-112.19391039999999</v>
       </c>
       <c r="AC81" s="2">
         <f t="shared" si="19"/>
@@ -11105,7 +11106,7 @@
       </c>
       <c r="AB82" s="2">
         <f t="shared" si="18"/>
-        <v>36.020554699999998</v>
+        <v>-112.19197339999999</v>
       </c>
       <c r="AC82" s="2">
         <f t="shared" si="19"/>
@@ -11214,7 +11215,7 @@
       </c>
       <c r="AB83" s="2">
         <f t="shared" si="18"/>
-        <v>36.061093800000002</v>
+        <v>-112.1743371</v>
       </c>
       <c r="AC83" s="2">
         <f t="shared" si="19"/>
@@ -11325,7 +11326,7 @@
       </c>
       <c r="AB84" s="2">
         <f t="shared" si="18"/>
-        <v>36.010086800000003</v>
+        <v>-112.31304660000001</v>
       </c>
       <c r="AC84" s="2">
         <f t="shared" si="19"/>
@@ -11434,7 +11435,7 @@
       </c>
       <c r="AB85" s="2">
         <f t="shared" si="18"/>
-        <v>36.083315499999998</v>
+        <v>-112.2285055</v>
       </c>
       <c r="AC85" s="2">
         <f t="shared" si="19"/>
@@ -11543,7 +11544,7 @@
       </c>
       <c r="AB86" s="2">
         <f t="shared" si="18"/>
-        <v>36.0710938</v>
+        <v>-112.1507254</v>
       </c>
       <c r="AC86" s="2">
         <f t="shared" si="19"/>
@@ -11652,7 +11653,7 @@
       </c>
       <c r="AB87" s="2">
         <f t="shared" si="18"/>
-        <v>36.102760000000004</v>
+        <v>-112.19517140000001</v>
       </c>
       <c r="AC87" s="2">
         <f t="shared" si="19"/>
@@ -11763,7 +11764,7 @@
       </c>
       <c r="AB88" s="2">
         <f t="shared" si="18"/>
-        <v>36.057482899999997</v>
+        <v>-112.13711379999999</v>
       </c>
       <c r="AC88" s="2">
         <f t="shared" si="19"/>
@@ -11873,7 +11874,7 @@
       </c>
       <c r="AB89" s="2">
         <f t="shared" si="18"/>
-        <v>36.010261</v>
+        <v>-112.2923959</v>
       </c>
       <c r="AC89" s="2">
         <f t="shared" si="19"/>
@@ -11982,7 +11983,7 @@
       </c>
       <c r="AB90" s="2">
         <f t="shared" si="18"/>
-        <v>36.048333300000003</v>
+        <v>-112.21972220000001</v>
       </c>
       <c r="AC90" s="2">
         <f t="shared" si="19"/>
@@ -12091,7 +12092,7 @@
       </c>
       <c r="AB91" s="2">
         <f t="shared" si="18"/>
-        <v>36.063611100000003</v>
+        <v>-112.1461111</v>
       </c>
       <c r="AC91" s="2">
         <f t="shared" si="19"/>
@@ -12202,7 +12203,7 @@
       </c>
       <c r="AB92" s="2">
         <f t="shared" si="18"/>
-        <v>36.049228100000001</v>
+        <v>-112.156629</v>
       </c>
       <c r="AC92" s="2">
         <f t="shared" si="19"/>
@@ -12311,7 +12312,7 @@
       </c>
       <c r="AB93" s="2">
         <f t="shared" si="18"/>
-        <v>36.057777799999997</v>
+        <v>-112.13666670000001</v>
       </c>
       <c r="AC93" s="2">
         <f t="shared" si="19"/>
@@ -12420,7 +12421,7 @@
       </c>
       <c r="AB94" s="2">
         <f t="shared" si="18"/>
-        <v>36.058055600000003</v>
+        <v>-112.1425</v>
       </c>
       <c r="AC94" s="2">
         <f t="shared" si="19"/>
@@ -12529,7 +12530,7 @@
       </c>
       <c r="AB95" s="2">
         <f t="shared" si="18"/>
-        <v>36.057222199999998</v>
+        <v>-112.1411111</v>
       </c>
       <c r="AC95" s="2">
         <f t="shared" si="19"/>
@@ -12638,7 +12639,7 @@
       </c>
       <c r="AB96" s="2">
         <f t="shared" si="18"/>
-        <v>36.107777800000001</v>
+        <v>-112.3133333</v>
       </c>
       <c r="AC96" s="2">
         <f t="shared" si="19"/>
@@ -12749,7 +12750,7 @@
       </c>
       <c r="AB97" s="2">
         <f t="shared" si="18"/>
-        <v>36.027483699999998</v>
+        <v>-112.18595550000001</v>
       </c>
       <c r="AC97" s="2">
         <f t="shared" si="19"/>
@@ -12860,7 +12861,7 @@
       </c>
       <c r="AB98" s="2">
         <f t="shared" si="18"/>
-        <v>36.052373000000003</v>
+        <v>-112.13865199999999</v>
       </c>
       <c r="AC98" s="2">
         <f t="shared" si="19"/>
@@ -12969,7 +12970,7 @@
       </c>
       <c r="AB99" s="2">
         <f t="shared" si="18"/>
-        <v>36.054495099999997</v>
+        <v>-112.1250879</v>
       </c>
       <c r="AC99" s="2">
         <f t="shared" si="19"/>

</xml_diff>